<commit_message>
Random problems and Med on AlgoExpert
</commit_message>
<xml_diff>
--- a/src/LeetCode Cheatsheet Excel.xlsx
+++ b/src/LeetCode Cheatsheet Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/IdeaProjects/LeetCode/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D5DE4B-BF70-924A-A151-EC50DC3FA044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F25FCB9-06C9-FA49-82E4-9CA2C626DA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="113">
   <si>
     <t>Serial Number</t>
   </si>
@@ -509,12 +509,31 @@
     <t>1. maintain return of left, right +1
 2. use recursion to increment left and right then pick Max</t>
   </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>1. for every match, increment indexes of both s1 and s2, if not, just increment s1
+2. compare s2 length and s2 count after loop ends</t>
+  </si>
+  <si>
+    <t>1. Maintain a left and right ptr, loop starts at 0, ends before I &lt; length-2
+3. if target = I + left + right, create new int[]
+4. if target &lt; sum then left ++, else target &gt; sum right--</t>
+  </si>
+  <si>
+    <t>Smallest Difference</t>
+  </si>
+  <si>
+    <t>1. Arrays.sort -&gt; Math.abs[A[a] - B[b]] &lt; result then result = diff and resultarr = new int {A[a], B[b]}
+2. if A &lt; B then a++ else b++</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -585,6 +604,12 @@
     <font>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFEFFFE"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -816,7 +841,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -890,6 +915,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2213,8 +2241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECCF676-020C-B847-B71D-4C6F1705BFB5}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2240,7 +2268,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -2250,10 +2278,12 @@
       <c r="C2" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="24" t="s">
+        <v>109</v>
+      </c>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -2263,18 +2293,30 @@
       <c r="C3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="25" t="s">
+        <v>110</v>
+      </c>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>112</v>
+      </c>
       <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -2574,10 +2616,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157F2540-6798-534A-9816-5C4E2978A222}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2743,6 +2785,17 @@
         <v>107</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Algo Expert Mediums and Trees Blind 150
</commit_message>
<xml_diff>
--- a/src/LeetCode Cheatsheet Excel.xlsx
+++ b/src/LeetCode Cheatsheet Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/IdeaProjects/LeetCode/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F25FCB9-06C9-FA49-82E4-9CA2C626DA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B82C05-7A1D-FB4A-B5F7-8CA2CDB25930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="121">
   <si>
     <t>Serial Number</t>
   </si>
@@ -481,9 +481,6 @@
 3. match cHead == cTail</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>1. loop each value
 2. maintain a minimun, if current &lt; min ; then current is min
 3. get profit = ip[i] - min; this needs to be maximum for every element in loop
@@ -527,13 +524,68 @@
   <si>
     <t>1. Arrays.sort -&gt; Math.abs[A[a] - B[b]] &lt; result then result = diff and resultarr = new int {A[a], B[b]}
 2. if A &lt; B then a++ else b++</t>
+  </si>
+  <si>
+    <t>1. Maintain a count for target match, ip[i] == target then count++
+2. else maintain a ptr to put all non target elements from 0 till length-1 - count
+3. another loop to reverse iterate and put target elements till length-1-count</t>
+  </si>
+  <si>
+    <t>Move Element to the End</t>
+  </si>
+  <si>
+    <t>Monotonic Array</t>
+  </si>
+  <si>
+    <t>1. maintain less and more counter, check counter == length-1 or not</t>
+  </si>
+  <si>
+    <t>Merge 2 sorted LL</t>
+  </si>
+  <si>
+    <t>Max value stock sell</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Iterative 2 pt prev next -&gt; create previous = null, while head is not null — next = head.next, head.next = previous, previous = head, head = next; +2. Recursive -&gt; fn(head, null) — </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>fn(head, previous)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> when head is null show previous +— next = head.next, head.next = previous — send fn(next, head)</t>
+    </r>
+  </si>
+  <si>
+    <t>Diameter of a Tree</t>
+  </si>
+  <si>
+    <t>1. call recursive maxDepth on root
+2. find maxDepth of left node, and right node
+3. increment +1 to the maxDepth of each left, righ section
+4. max = left+right, max -&gt; Math.max - max to keep count of max depth of each left right node travel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -613,8 +665,21 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -636,6 +701,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,7 +912,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -918,6 +989,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1261,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A304D053-03E3-634E-ACC7-B3F757D9248A}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2241,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECCF676-020C-B847-B71D-4C6F1705BFB5}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2279,7 +2353,7 @@
         <v>95</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E2" s="22"/>
     </row>
@@ -2294,7 +2368,7 @@
         <v>96</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" s="22"/>
     </row>
@@ -2306,27 +2380,41 @@
         <v>18</v>
       </c>
       <c r="C4" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>112</v>
-      </c>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="22">
         <v>4</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="B5" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>112</v>
+      </c>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>115</v>
+      </c>
       <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2616,10 +2704,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157F2540-6798-534A-9816-5C4E2978A222}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2712,10 +2800,10 @@
         <v>92</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>101</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="56" x14ac:dyDescent="0.15">
@@ -2729,7 +2817,7 @@
         <v>76</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="56" x14ac:dyDescent="0.15">
@@ -2743,7 +2831,7 @@
         <v>97</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.15">
@@ -2757,7 +2845,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -2779,13 +2867,13 @@
         <v>98</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:5" ht="98" x14ac:dyDescent="0.15">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -2793,7 +2881,38 @@
         <v>39</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A13" s="16">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="98" x14ac:dyDescent="0.15">
+      <c r="A14" s="16">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>